<commit_message>
Fix test after adding new name restrictions in ODK Tools
</commit_message>
<xml_diff>
--- a/formshare/tests/resources/forms/merge_multilanguaje/asistencia_tecnica.xlsx
+++ b/formshare/tests/resources/forms/merge_multilanguaje/asistencia_tecnica.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" state="visible" r:id="rId2"/>
@@ -63,7 +63,7 @@
     <t xml:space="preserve">end</t>
   </si>
   <si>
-    <t xml:space="preserve">final</t>
+    <t xml:space="preserve">fe_final</t>
   </si>
   <si>
     <t xml:space="preserve">today</t>
@@ -367,8 +367,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -391,216 +395,216 @@
   </sheetPr>
   <dimension ref="A1:J13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F21" activeCellId="1" sqref="C1:C2 F21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="0" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="0" t="s">
+      <c r="E6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="0" t="s">
+      <c r="F6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="0" t="s">
+      <c r="G6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="0" t="s">
+      <c r="H6" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="0" t="s">
+      <c r="E7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="0" t="s">
+      <c r="G7" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="G8" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="0" t="s">
+      <c r="E9" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G9" s="0" t="s">
+      <c r="G9" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G10" s="0" t="s">
+      <c r="G10" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="0" t="s">
+      <c r="E11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G11" s="0" t="s">
+      <c r="G11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I11" s="0" t="s">
+      <c r="I11" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="0" t="s">
+      <c r="G12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J12" s="0" t="s">
+      <c r="J12" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="0" t="s">
+      <c r="B13" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J13" s="0" t="s">
+      <c r="J13" s="1" t="s">
         <v>46</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -616,425 +620,425 @@
   <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="1" sqref="C1:C2 B2"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B2" s="0" t="s">
+      <c r="A2" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3" s="0" t="s">
+      <c r="A3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B4" s="0" t="s">
+      <c r="A4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B5" s="0" t="s">
+      <c r="A5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B6" s="0" t="s">
+      <c r="A6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="0" t="s">
+      <c r="A7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="0" t="s">
+      <c r="A8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" s="0" t="s">
+      <c r="A9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="0" t="s">
+      <c r="A10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" s="0" t="s">
+      <c r="A11" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="1" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="0" t="s">
+      <c r="A12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="1" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="0" t="s">
+      <c r="A13" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="C13" s="1" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="0" t="s">
+      <c r="A14" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="C14" s="1" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B15" s="0" t="s">
+      <c r="A15" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="C15" s="1" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B16" s="0" t="s">
+      <c r="A16" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="C16" s="1" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" s="0" t="s">
+      <c r="A17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="0" t="s">
+      <c r="C17" s="1" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B18" s="0" t="s">
+      <c r="A18" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="C18" s="1" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B19" s="0" t="s">
+      <c r="A19" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="C19" s="1" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B20" s="0" t="s">
+      <c r="A20" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="C20" s="1" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B21" s="0" t="s">
+      <c r="A21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="C21" s="1" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" s="0" t="s">
+      <c r="A22" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="C22" s="1" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B23" s="0" t="s">
+      <c r="A23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="C23" s="1" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B24" s="0" t="s">
+      <c r="A24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="C24" s="1" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B25" s="0" t="s">
+      <c r="A25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="C25" s="1" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B26" s="0" t="s">
+      <c r="A26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="C26" s="0" t="s">
+      <c r="C26" s="1" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B27" s="0" t="s">
+      <c r="A27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C27" s="0" t="s">
+      <c r="C27" s="1" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B28" s="0" t="s">
+      <c r="A28" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B28" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C28" s="0" t="s">
+      <c r="C28" s="1" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="0" t="s">
+      <c r="A29" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C29" s="0" t="s">
+      <c r="C29" s="1" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B30" s="0" t="s">
+      <c r="A30" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B30" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="C30" s="0" t="s">
+      <c r="C30" s="1" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B31" s="0" t="s">
+      <c r="A31" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C31" s="0" t="s">
+      <c r="C31" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B32" s="0" t="s">
+      <c r="A32" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="C32" s="0" t="s">
+      <c r="C32" s="1" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B33" s="0" t="s">
+      <c r="A33" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C33" s="0" t="s">
+      <c r="C33" s="1" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B34" s="0" t="s">
+      <c r="A34" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C34" s="0" t="s">
+      <c r="C34" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B35" s="0" t="s">
+      <c r="A35" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C35" s="0" t="s">
+      <c r="C35" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B36" s="0" t="s">
+      <c r="A36" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C36" s="0" t="s">
+      <c r="C36" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B37" s="0" t="s">
+      <c r="A37" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="C37" s="0" t="s">
+      <c r="C37" s="1" t="s">
         <v>84</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1049,35 +1053,35 @@
   </sheetPr>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1:C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.59375" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>89</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>